<commit_message>
Diapositivas, informe, imagenes - HyS
</commit_message>
<xml_diff>
--- a/Seguridad-Higiene/Matafuegos.xlsx
+++ b/Seguridad-Higiene/Matafuegos.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="43">
   <si>
     <t>Piso</t>
   </si>
@@ -99,9 +99,6 @@
     <t>Área Digital</t>
   </si>
   <si>
-    <t>Kitchenete</t>
-  </si>
-  <si>
     <t>Tercer Piso</t>
   </si>
   <si>
@@ -142,6 +139,12 @@
   </si>
   <si>
     <t>Entrevistas</t>
+  </si>
+  <si>
+    <t>Escaleras</t>
+  </si>
+  <si>
+    <t>Sala de Reuniones</t>
   </si>
 </sst>
 </file>
@@ -197,7 +200,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -257,17 +260,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -278,6 +292,11 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -287,11 +306,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -593,10 +608,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:H27"/>
+  <dimension ref="A3:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -612,278 +627,357 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="9" t="s">
-        <v>35</v>
+      <c r="B4" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>39</v>
+        <v>5</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="5"/>
+      <c r="E4" s="4">
+        <v>5</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="5"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="6" t="s">
+      <c r="D7" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="E6" s="6"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="11"/>
-      <c r="C7" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="6"/>
+      <c r="E7" s="4">
+        <v>2</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" s="12"/>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="13"/>
+      <c r="C9" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D9" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="6"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" s="6"/>
+      <c r="E9" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="6"/>
+      <c r="D10" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="11"/>
-      <c r="C11" s="6" t="s">
+      <c r="B11" s="12"/>
+      <c r="C11" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" s="6"/>
+      <c r="D11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="12"/>
-      <c r="C12" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" s="6" t="s">
+      <c r="B12" s="13"/>
+      <c r="C12" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E12" s="6"/>
+      <c r="E12" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" s="6"/>
+      <c r="D13" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="4">
+        <v>2</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="11"/>
-      <c r="C14" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" s="6"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" s="12"/>
-      <c r="C15" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D15" s="6" t="s">
+      <c r="C15" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E15" s="6"/>
+      <c r="E15" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E16" s="6"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="11"/>
-      <c r="C17" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E17" s="6"/>
+      <c r="B17" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="4">
+        <v>2</v>
+      </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="12"/>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D18" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" s="13"/>
+      <c r="C19" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E18" s="6"/>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B19" s="10" t="s">
+      <c r="E19" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="D20" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="12"/>
+      <c r="C21" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E21" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="13"/>
+      <c r="C22" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="D19" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E19" s="6"/>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="12"/>
-      <c r="C20" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D20" s="6" t="s">
+      <c r="C23" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24" s="12"/>
+      <c r="C24" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E20" s="6"/>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E21" s="6"/>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="G22" s="14" t="s">
+      <c r="E24" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="13"/>
+      <c r="C25" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E25" s="4">
+        <v>1</v>
+      </c>
+      <c r="G25" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="H22" s="14" t="s">
+      <c r="H25" s="9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="G23" s="15" t="s">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G26" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="H23" s="3" t="s">
+      <c r="H26" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="G24" s="15" t="s">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G27" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="H24" s="3" t="s">
+      <c r="H27" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="G25" s="15" t="s">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G28" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="H25" s="3" t="s">
+      <c r="H28" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="G26" s="15" t="s">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G29" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="H26" s="3" t="s">
+      <c r="H29" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="G27" s="15" t="s">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G30" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="H27" s="3" t="s">
+      <c r="H30" s="2" t="s">
         <v>17</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="B6:B8"/>
+  <mergeCells count="6">
+    <mergeCell ref="B23:B25"/>
     <mergeCell ref="B10:B12"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="B16:B18"/>
-    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="B20:B22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Subo todo lo que hizo la Yami!!!
</commit_message>
<xml_diff>
--- a/Seguridad-Higiene/Matafuegos.xlsx
+++ b/Seguridad-Higiene/Matafuegos.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="45">
   <si>
     <t>Piso</t>
   </si>
@@ -33,9 +33,6 @@
     <t>Clase K</t>
   </si>
   <si>
-    <t>Expedición</t>
-  </si>
-  <si>
     <t>Clase ABC</t>
   </si>
   <si>
@@ -145,6 +142,15 @@
   </si>
   <si>
     <t>Sala de Reuniones</t>
+  </si>
+  <si>
+    <t>Depósito Producción</t>
+  </si>
+  <si>
+    <t>Depósito Expedición</t>
+  </si>
+  <si>
+    <t>Producción</t>
   </si>
 </sst>
 </file>
@@ -200,7 +206,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -273,11 +279,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -292,11 +318,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -306,7 +330,12 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -608,10 +637,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:H30"/>
+  <dimension ref="A3:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -637,112 +666,110 @@
         <v>3</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="8" t="s">
-        <v>18</v>
+      <c r="B4" s="11" t="s">
+        <v>17</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>6</v>
-      </c>
       <c r="E4" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="12"/>
+      <c r="C5" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="7" t="s">
+      <c r="E5" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="12"/>
+      <c r="C6" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="13"/>
+      <c r="C7" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D7" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E7" s="4">
+      <c r="D9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="3">
         <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="12"/>
-      <c r="C8" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="13"/>
-      <c r="C9" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" s="4">
-        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" s="11" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="E10" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" s="12"/>
       <c r="C11" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E11" s="4">
         <v>1</v>
@@ -751,10 +778,10 @@
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" s="13"/>
       <c r="C12" s="4" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E12" s="4">
         <v>1</v>
@@ -762,25 +789,25 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" s="11" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E13" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" s="12"/>
       <c r="C14" s="4" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E14" s="4">
         <v>1</v>
@@ -789,7 +816,7 @@
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" s="12"/>
       <c r="C15" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>4</v>
@@ -801,10 +828,10 @@
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" s="13"/>
       <c r="C16" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E16" s="4">
         <v>1</v>
@@ -812,34 +839,34 @@
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="11" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E17" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="12"/>
       <c r="C18" s="4" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E18" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B19" s="13"/>
+      <c r="B19" s="12"/>
       <c r="C19" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>4</v>
@@ -849,135 +876,208 @@
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="13"/>
+      <c r="C20" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="12"/>
+      <c r="C22" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="12"/>
+      <c r="C23" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E23" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24" s="13"/>
+      <c r="C24" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E24" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="D25" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E25" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B26" s="12"/>
+      <c r="C26" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E26" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="13"/>
+      <c r="C27" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E27" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B28" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="C28" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E28" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B29" s="15"/>
+      <c r="C29" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E29" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B30" s="15"/>
+      <c r="C30" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E30" s="4">
+        <v>1</v>
+      </c>
+      <c r="G30" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="H30" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B31" s="15"/>
+      <c r="C31" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E31" s="4">
+        <v>1</v>
+      </c>
+      <c r="G31" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G32" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E20" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="12"/>
-      <c r="C21" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E21" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="13"/>
-      <c r="C22" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E22" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E23" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="12"/>
-      <c r="C24" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E24" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="13"/>
-      <c r="C25" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E25" s="4">
-        <v>1</v>
-      </c>
-      <c r="G25" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="H25" s="9" t="s">
+      <c r="H32" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="G26" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="G27" s="10" t="s">
+    <row r="33" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G33" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="H27" s="2" t="s">
+      <c r="H33" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="G28" s="10" t="s">
+    <row r="34" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G34" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H28" s="2" t="s">
+      <c r="H34" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G35" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H35" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="G29" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="G30" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="H30" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="B23:B25"/>
+  <mergeCells count="7">
+    <mergeCell ref="B4:B7"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="B21:B24"/>
+    <mergeCell ref="B28:B31"/>
     <mergeCell ref="B10:B12"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="B13:B16"/>
-    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="B17:B20"/>
+    <mergeCell ref="B25:B27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>